<commit_message>
new app invoicing added to send emails
</commit_message>
<xml_diff>
--- a/Tracking Details.xlsx
+++ b/Tracking Details.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ups</t>
+          <t>UPS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -470,7 +470,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ups</t>
+          <t>UPS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -487,7 +487,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ups</t>
+          <t>UPS</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>

<commit_message>
updated the html designs
</commit_message>
<xml_diff>
--- a/Tracking Details.xlsx
+++ b/Tracking Details.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
added links for other carriers
</commit_message>
<xml_diff>
--- a/Tracking Details.xlsx
+++ b/Tracking Details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +501,38 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FASTFRATE</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1061743489</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DAYROSS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>VAN64300833</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>